<commit_message>
added different years to data and added slider to view
</commit_message>
<xml_diff>
--- a/data/fullTable.xlsx
+++ b/data/fullTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joelm\Documents\FHNW\_IVIS\IVISPro\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\WebstormProjects\FootballClubEfficiency\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="238">
   <si>
     <t>Platzierung</t>
   </si>
@@ -994,6 +994,30 @@
   </si>
   <si>
     <t>3772,32</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>Umsatz</t>
+  </si>
+  <si>
+    <t>http://fussball-geld.de/umsatz-der-bundesligisten-in-der-saison-20152016/</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2013</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1095,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1090,8 +1114,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1206,12 +1236,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1280,6 +1321,14 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1595,10 +1644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,10 +1656,11 @@
     <col min="4" max="4" width="18.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="3"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1629,11 +1679,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1652,11 +1705,12 @@
       <c r="F2" s="5">
         <v>14.55</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="26"/>
+      <c r="H2" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>35</v>
       </c>
@@ -1675,11 +1729,12 @@
       <c r="F3" s="5">
         <v>7.85</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="26"/>
+      <c r="H3" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>32</v>
       </c>
@@ -1698,11 +1753,12 @@
       <c r="F4" s="5">
         <v>6.11</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="26"/>
+      <c r="H4" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>37</v>
       </c>
@@ -1721,11 +1777,12 @@
       <c r="F5" s="5">
         <v>3.54</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="26"/>
+      <c r="H5" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
@@ -1744,11 +1801,12 @@
       <c r="F6" s="5">
         <v>3.62</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="26"/>
+      <c r="H6" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>38</v>
       </c>
@@ -1767,11 +1825,14 @@
       <c r="F7" s="5">
         <v>3.95</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G7" s="26">
+        <v>116.7</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>25</v>
       </c>
@@ -1790,11 +1851,12 @@
       <c r="F8" s="5">
         <v>3.19</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="26"/>
+      <c r="H8" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>28</v>
       </c>
@@ -1813,11 +1875,12 @@
       <c r="F9" s="5">
         <v>2.75</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="26"/>
+      <c r="H9" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>27</v>
       </c>
@@ -1836,11 +1899,12 @@
       <c r="F10" s="5">
         <v>2.02</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="26"/>
+      <c r="H10" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -1859,11 +1923,12 @@
       <c r="F11" s="5">
         <v>3</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="26"/>
+      <c r="H11" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>29</v>
       </c>
@@ -1882,11 +1947,12 @@
       <c r="F12" s="5">
         <v>2.48</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="26"/>
+      <c r="H12" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>33</v>
       </c>
@@ -1905,11 +1971,14 @@
       <c r="F13" s="5">
         <v>1.65</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="26">
+        <v>58.76</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>36</v>
       </c>
@@ -1928,11 +1997,12 @@
       <c r="F14" s="5">
         <v>1.64</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="26"/>
+      <c r="H14" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>30</v>
       </c>
@@ -1951,11 +2021,12 @@
       <c r="F15" s="5">
         <v>1.52</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="26"/>
+      <c r="H15" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>31</v>
       </c>
@@ -1974,11 +2045,14 @@
       <c r="F16" s="5">
         <v>1.47</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="26">
+        <v>50</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>26</v>
       </c>
@@ -1997,11 +2071,12 @@
       <c r="F17" s="5">
         <v>1.42</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="26"/>
+      <c r="H17" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>40</v>
       </c>
@@ -2020,11 +2095,12 @@
       <c r="F18" s="5">
         <v>0.92100000000000004</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="26"/>
+      <c r="H18" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>39</v>
       </c>
@@ -2043,11 +2119,12 @@
       <c r="F19" s="5">
         <v>0.93400000000000005</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="26"/>
+      <c r="H19" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>1</v>
       </c>
@@ -2066,11 +2143,12 @@
       <c r="F20" s="7">
         <v>16.13</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="27"/>
+      <c r="H20" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>2</v>
       </c>
@@ -2089,11 +2167,14 @@
       <c r="F21" s="7">
         <v>9.1999999999999993</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="27">
+        <v>260.7</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>3</v>
       </c>
@@ -2112,11 +2193,12 @@
       <c r="F22" s="7">
         <v>5.67</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G22" s="27"/>
+      <c r="H22" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>4</v>
       </c>
@@ -2135,11 +2217,12 @@
       <c r="F23" s="7">
         <v>4.3</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G23" s="27"/>
+      <c r="H23" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>5</v>
       </c>
@@ -2158,11 +2241,12 @@
       <c r="F24" s="7">
         <v>3.85</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G24" s="27"/>
+      <c r="H24" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>16</v>
       </c>
@@ -2181,11 +2265,14 @@
       <c r="F25" s="7">
         <v>3.38</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G25" s="27">
+        <v>121.1</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>15</v>
       </c>
@@ -2204,11 +2291,12 @@
       <c r="F26" s="7">
         <v>3.16</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="27"/>
+      <c r="H26" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>6</v>
       </c>
@@ -2227,11 +2315,12 @@
       <c r="F27" s="7">
         <v>3.38</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="27"/>
+      <c r="H27" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>13</v>
       </c>
@@ -2250,11 +2339,14 @@
       <c r="F28" s="7">
         <v>2.57</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="27">
+        <v>99</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>10</v>
       </c>
@@ -2273,11 +2365,12 @@
       <c r="F29" s="7">
         <v>2.39</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="27"/>
+      <c r="H29" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>9</v>
       </c>
@@ -2296,11 +2389,12 @@
       <c r="F30" s="7">
         <v>1.79</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="27"/>
+      <c r="H30" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>12</v>
       </c>
@@ -2319,11 +2413,12 @@
       <c r="F31" s="7">
         <v>1.96</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="27"/>
+      <c r="H31" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>14</v>
       </c>
@@ -2342,11 +2437,14 @@
       <c r="F32" s="7">
         <v>1.96</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G32" s="27">
+        <v>70</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>17</v>
       </c>
@@ -2365,11 +2463,12 @@
       <c r="F33" s="7">
         <v>1.53</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G33" s="27"/>
+      <c r="H33" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
         <v>11</v>
       </c>
@@ -2388,11 +2487,14 @@
       <c r="F34" s="7">
         <v>1.44</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="27">
+        <v>104.3</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>7</v>
       </c>
@@ -2411,11 +2513,12 @@
       <c r="F35" s="7">
         <v>1.46</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G35" s="27"/>
+      <c r="H35" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>8</v>
       </c>
@@ -2434,11 +2537,12 @@
       <c r="F36" s="7">
         <v>1.28</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G36" s="27"/>
+      <c r="H36" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>18</v>
       </c>
@@ -2457,11 +2561,12 @@
       <c r="F37" s="7">
         <v>0.92500000000000004</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G37" s="27"/>
+      <c r="H37" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>1</v>
       </c>
@@ -2480,11 +2585,14 @@
       <c r="F38" s="7">
         <v>17.100000000000001</v>
       </c>
-      <c r="G38" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G38" s="27">
+        <v>523.70000000000005</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8">
         <v>7</v>
       </c>
@@ -2503,11 +2611,14 @@
       <c r="F39" s="7">
         <v>8.91</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G39" s="27">
+        <v>276</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <v>6</v>
       </c>
@@ -2526,11 +2637,14 @@
       <c r="F40" s="7">
         <v>5.93</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G40" s="27">
+        <v>255.7</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
         <v>2</v>
       </c>
@@ -2549,11 +2663,14 @@
       <c r="F41" s="7">
         <v>5.87</v>
       </c>
-      <c r="G41" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G41" s="27">
+        <v>250</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="8">
         <v>4</v>
       </c>
@@ -2572,11 +2689,14 @@
       <c r="F42" s="7">
         <v>6.41</v>
       </c>
-      <c r="G42" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G42" s="27">
+        <v>200</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <v>16</v>
       </c>
@@ -2595,11 +2715,14 @@
       <c r="F43" s="7">
         <v>3.03</v>
       </c>
-      <c r="G43" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G43" s="27">
+        <v>128.1</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8">
         <v>3</v>
       </c>
@@ -2618,11 +2741,14 @@
       <c r="F44" s="7">
         <v>3.98</v>
       </c>
-      <c r="G44" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G44" s="27">
+        <v>130.6</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8">
         <v>8</v>
       </c>
@@ -2641,11 +2767,14 @@
       <c r="F45" s="7">
         <v>3.33</v>
       </c>
-      <c r="G45" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G45" s="27">
+        <v>71.5</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8">
         <v>14</v>
       </c>
@@ -2664,11 +2793,14 @@
       <c r="F46" s="7">
         <v>3.26</v>
       </c>
-      <c r="G46" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G46" s="27">
+        <v>119</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>13</v>
       </c>
@@ -2687,11 +2819,14 @@
       <c r="F47" s="7">
         <v>2.23</v>
       </c>
-      <c r="G47" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G47" s="27">
+        <v>68.13</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="8">
         <v>11</v>
       </c>
@@ -2710,11 +2845,14 @@
       <c r="F48" s="7">
         <v>2.14</v>
       </c>
-      <c r="G48" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G48" s="27">
+        <v>75.3</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
         <v>15</v>
       </c>
@@ -2733,11 +2871,14 @@
       <c r="F49" s="7">
         <v>2.5499999999999998</v>
       </c>
-      <c r="G49" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G49" s="27">
+        <v>88.5</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
         <v>9</v>
       </c>
@@ -2756,11 +2897,14 @@
       <c r="F50" s="7">
         <v>2.4700000000000002</v>
       </c>
-      <c r="G50" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G50" s="27">
+        <v>66.7</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8">
         <v>10</v>
       </c>
@@ -2779,11 +2923,14 @@
       <c r="F51" s="7">
         <v>1.63</v>
       </c>
-      <c r="G51" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G51" s="27">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8">
         <v>17</v>
       </c>
@@ -2802,11 +2949,14 @@
       <c r="F52" s="7">
         <v>1.9</v>
       </c>
-      <c r="G52" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G52" s="27">
+        <v>68.34</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="8">
         <v>12</v>
       </c>
@@ -2825,11 +2975,14 @@
       <c r="F53" s="7">
         <v>1.6</v>
       </c>
-      <c r="G53" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G53" s="27">
+        <v>89.7</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8">
         <v>5</v>
       </c>
@@ -2848,11 +3001,14 @@
       <c r="F54" s="7">
         <v>1.21</v>
       </c>
-      <c r="G54" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G54" s="27">
+        <v>59.38</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="8">
         <v>18</v>
       </c>
@@ -2871,11 +3027,14 @@
       <c r="F55" s="7">
         <v>0.80200000000000005</v>
       </c>
-      <c r="G55" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G55" s="27">
+        <v>29.83</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8">
         <v>1</v>
       </c>
@@ -2894,11 +3053,17 @@
       <c r="F56" s="7">
         <v>17.899999999999999</v>
       </c>
-      <c r="G56" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G56" s="27">
+        <v>626.79999999999995</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="J56" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="8">
         <v>2</v>
       </c>
@@ -2917,11 +3082,14 @@
       <c r="F57" s="7">
         <v>10.39</v>
       </c>
-      <c r="G57" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G57" s="27">
+        <v>376.3</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8">
         <v>8</v>
       </c>
@@ -2940,11 +3108,14 @@
       <c r="F58" s="7">
         <v>7.58</v>
       </c>
-      <c r="G58" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G58" s="27">
+        <v>240</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8">
         <v>5</v>
       </c>
@@ -2963,11 +3134,14 @@
       <c r="F59" s="7">
         <v>6.54</v>
       </c>
-      <c r="G59" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G59" s="27">
+        <v>264.5</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="8">
         <v>3</v>
       </c>
@@ -2986,11 +3160,14 @@
       <c r="F60" s="7">
         <v>6.08</v>
       </c>
-      <c r="G60" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G60" s="27">
+        <v>236.1</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8">
         <v>4</v>
       </c>
@@ -3009,11 +3186,14 @@
       <c r="F61" s="7">
         <v>4.8099999999999996</v>
       </c>
-      <c r="G61" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G61" s="27">
+        <v>160.6</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="8">
         <v>15</v>
       </c>
@@ -3032,11 +3212,14 @@
       <c r="F62" s="7">
         <v>3.59</v>
       </c>
-      <c r="G62" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G62" s="27">
+        <v>128</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="8">
         <v>16</v>
       </c>
@@ -3055,11 +3238,14 @@
       <c r="F63" s="7">
         <v>2.5</v>
       </c>
-      <c r="G63" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G63" s="27">
+        <v>104</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="8">
         <v>17</v>
       </c>
@@ -3078,11 +3264,14 @@
       <c r="F64" s="7">
         <v>2.4300000000000002</v>
       </c>
-      <c r="G64" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G64" s="27">
+        <v>125.5</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="8">
         <v>10</v>
       </c>
@@ -3101,11 +3290,14 @@
       <c r="F65" s="7">
         <v>2.12</v>
       </c>
-      <c r="G65" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G65" s="27">
+        <v>123</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8">
         <v>18</v>
       </c>
@@ -3124,11 +3316,14 @@
       <c r="F66" s="7">
         <v>1.89</v>
       </c>
-      <c r="G66" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G66" s="27">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="8">
         <v>7</v>
       </c>
@@ -3147,11 +3342,14 @@
       <c r="F67" s="7">
         <v>2.14</v>
       </c>
-      <c r="G67" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G67" s="27">
+        <v>95.2</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="8">
         <v>6</v>
       </c>
@@ -3170,11 +3368,14 @@
       <c r="F68" s="7">
         <v>1.73</v>
       </c>
-      <c r="G68" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G68" s="27">
+        <v>104.8</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="8">
         <v>12</v>
       </c>
@@ -3193,11 +3394,14 @@
       <c r="F69" s="7">
         <v>1.6</v>
       </c>
-      <c r="G69" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G69" s="27">
+        <v>96.3</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="8">
         <v>13</v>
       </c>
@@ -3216,11 +3420,14 @@
       <c r="F70" s="7">
         <v>1.53</v>
       </c>
-      <c r="G70" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G70" s="27">
+        <v>108.1</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="8">
         <v>9</v>
       </c>
@@ -3239,11 +3446,14 @@
       <c r="F71" s="7">
         <v>2.08</v>
       </c>
-      <c r="G71" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G71" s="27">
+        <v>107</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="8">
         <v>11</v>
       </c>
@@ -3262,11 +3472,14 @@
       <c r="F72" s="7">
         <v>0.84099999999999997</v>
       </c>
-      <c r="G72" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G72" s="27">
+        <v>54.3</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="8">
         <v>14</v>
       </c>
@@ -3285,11 +3498,14 @@
       <c r="F73" s="7">
         <v>0.66</v>
       </c>
-      <c r="G73" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G73" s="27">
+        <v>41.5</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="8">
         <v>1</v>
       </c>
@@ -3308,11 +3524,14 @@
       <c r="F74" s="7">
         <v>18.04</v>
       </c>
-      <c r="G74" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G74" s="28">
+        <v>640.5</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="8">
         <v>3</v>
       </c>
@@ -3331,11 +3550,14 @@
       <c r="F75" s="7">
         <v>10.36</v>
       </c>
-      <c r="G75" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G75" s="29">
+        <v>405.7</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="8">
         <v>12</v>
       </c>
@@ -3354,11 +3576,14 @@
       <c r="F76" s="7">
         <v>6.27</v>
       </c>
-      <c r="G76" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G76" s="28">
+        <v>203.8</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="8">
         <v>10</v>
       </c>
@@ -3377,11 +3602,14 @@
       <c r="F77" s="7">
         <v>6.12</v>
       </c>
-      <c r="G77" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G77" s="29">
+        <v>256.10000000000002</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="8">
         <v>16</v>
       </c>
@@ -3400,11 +3628,14 @@
       <c r="F78" s="7">
         <v>5.24</v>
       </c>
-      <c r="G78" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G78" s="28">
+        <v>190</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="8">
         <v>9</v>
       </c>
@@ -3423,11 +3654,14 @@
       <c r="F79" s="7">
         <v>4.72</v>
       </c>
-      <c r="G79" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G79" s="29">
+        <v>196.9</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="8">
         <v>14</v>
       </c>
@@ -3446,11 +3680,14 @@
       <c r="F80" s="7">
         <v>2.5</v>
       </c>
-      <c r="G80" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G80" s="28">
+        <v>122.1</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8">
         <v>15</v>
       </c>
@@ -3469,11 +3706,14 @@
       <c r="F81" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G81" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G81" s="29">
+        <v>110.1</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="8">
         <v>5</v>
       </c>
@@ -3492,11 +3732,14 @@
       <c r="F82" s="7">
         <v>2.58</v>
       </c>
-      <c r="G82" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G82" s="28">
+        <v>129</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="8">
         <v>4</v>
       </c>
@@ -3515,11 +3758,14 @@
       <c r="F83" s="7">
         <v>2.3199999999999998</v>
       </c>
-      <c r="G83" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G83" s="29">
+        <v>111</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="8">
         <v>6</v>
       </c>
@@ -3538,11 +3784,14 @@
       <c r="F84" s="7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G84" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G84" s="28">
+        <v>112.3</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="8">
         <v>8</v>
       </c>
@@ -3561,11 +3810,14 @@
       <c r="F85" s="7">
         <v>1.83</v>
       </c>
-      <c r="G85" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G85" s="29">
+        <v>123.5</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="8">
         <v>2</v>
       </c>
@@ -3584,11 +3836,14 @@
       <c r="F86" s="7">
         <v>2.1</v>
       </c>
-      <c r="G86" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G86" s="28">
+        <v>205</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="8">
         <v>13</v>
       </c>
@@ -3607,11 +3862,14 @@
       <c r="F87" s="7">
         <v>1.86</v>
       </c>
-      <c r="G87" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G87" s="29">
+        <v>94.8</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="8">
         <v>11</v>
       </c>
@@ -3630,11 +3888,14 @@
       <c r="F88" s="7">
         <v>1.89</v>
       </c>
-      <c r="G88" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G88" s="28">
+        <v>109.2</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="8">
         <v>7</v>
       </c>
@@ -3653,11 +3914,14 @@
       <c r="F89" s="7">
         <v>1.1200000000000001</v>
       </c>
-      <c r="G89" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G89" s="29">
+        <v>63</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="8">
         <v>17</v>
       </c>
@@ -3676,11 +3940,14 @@
       <c r="F90" s="7">
         <v>1.1499999999999999</v>
       </c>
-      <c r="G90" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G90" s="28">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="8">
         <v>18</v>
       </c>
@@ -3699,11 +3966,14 @@
       <c r="F91" s="7">
         <v>0.84199999999999997</v>
       </c>
-      <c r="G91" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G91" s="29">
+        <v>47.8</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="8">
         <v>1</v>
       </c>
@@ -3722,11 +3992,12 @@
       <c r="F92" s="7">
         <v>28.85</v>
       </c>
-      <c r="G92" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G92" s="28"/>
+      <c r="H92" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="8">
         <v>3</v>
       </c>
@@ -3745,11 +4016,12 @@
       <c r="F93" s="7">
         <v>14.46</v>
       </c>
-      <c r="G93" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G93" s="29"/>
+      <c r="H93" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="8">
         <v>6</v>
       </c>
@@ -3768,11 +4040,12 @@
       <c r="F94" s="7">
         <v>14.65</v>
       </c>
-      <c r="G94" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G94" s="28"/>
+      <c r="H94" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="8">
         <v>4</v>
       </c>
@@ -3791,11 +4064,12 @@
       <c r="F95" s="7">
         <v>13.41</v>
       </c>
-      <c r="G95" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G95" s="29"/>
+      <c r="H95" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="8">
         <v>2</v>
       </c>
@@ -3814,11 +4088,12 @@
       <c r="F96" s="7">
         <v>9.65</v>
       </c>
-      <c r="G96" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G96" s="28"/>
+      <c r="H96" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="8">
         <v>8</v>
       </c>
@@ -3837,11 +4112,12 @@
       <c r="F97" s="7">
         <v>7.23</v>
       </c>
-      <c r="G97" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G97" s="29"/>
+      <c r="H97" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="8">
         <v>5</v>
       </c>
@@ -3860,11 +4136,12 @@
       <c r="F98" s="7">
         <v>5.64</v>
       </c>
-      <c r="G98" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G98" s="28"/>
+      <c r="H98" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="8">
         <v>14</v>
       </c>
@@ -3883,11 +4160,12 @@
       <c r="F99" s="7">
         <v>4.93</v>
       </c>
-      <c r="G99" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G99" s="29"/>
+      <c r="H99" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="8">
         <v>9</v>
       </c>
@@ -3906,11 +4184,12 @@
       <c r="F100" s="7">
         <v>4.25</v>
       </c>
-      <c r="G100" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G100" s="28"/>
+      <c r="H100" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="8">
         <v>18</v>
       </c>
@@ -3929,11 +4208,12 @@
       <c r="F101" s="7">
         <v>3.57</v>
       </c>
-      <c r="G101" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G101" s="29"/>
+      <c r="H101" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="8">
         <v>7</v>
       </c>
@@ -3952,11 +4232,12 @@
       <c r="F102" s="7">
         <v>3.46</v>
       </c>
-      <c r="G102" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G102" s="28"/>
+      <c r="H102" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="8">
         <v>10</v>
       </c>
@@ -3975,11 +4256,12 @@
       <c r="F103" s="7">
         <v>4.12</v>
       </c>
-      <c r="G103" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G103" s="29"/>
+      <c r="H103" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="8">
         <v>12</v>
       </c>
@@ -3998,11 +4280,12 @@
       <c r="F104" s="7">
         <v>2.99</v>
       </c>
-      <c r="G104" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G104" s="28"/>
+      <c r="H104" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="8">
         <v>16</v>
       </c>
@@ -4021,11 +4304,12 @@
       <c r="F105" s="7">
         <v>2.6</v>
       </c>
-      <c r="G105" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G105" s="29"/>
+      <c r="H105" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="8">
         <v>11</v>
       </c>
@@ -4044,11 +4328,12 @@
       <c r="F106" s="7">
         <v>3.31</v>
       </c>
-      <c r="G106" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G106" s="28"/>
+      <c r="H106" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="8">
         <v>13</v>
       </c>
@@ -4067,11 +4352,12 @@
       <c r="F107" s="7">
         <v>2.93</v>
       </c>
-      <c r="G107" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G107" s="29"/>
+      <c r="H107" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="8">
         <v>15</v>
       </c>
@@ -4090,11 +4376,12 @@
       <c r="F108" s="7">
         <v>3.28</v>
       </c>
-      <c r="G108" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G108" s="28"/>
+      <c r="H108" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="8">
         <v>17</v>
       </c>
@@ -4113,8 +4400,9 @@
       <c r="F109" s="7">
         <v>2.17</v>
       </c>
-      <c r="G109" s="3" t="s">
-        <v>65</v>
+      <c r="G109" s="29"/>
+      <c r="H109" s="3" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>